<commit_message>
top interview last 20
</commit_message>
<xml_diff>
--- a/leetcode/leetcode_divide_conquer.xlsx
+++ b/leetcode/leetcode_divide_conquer.xlsx
@@ -3,14 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A959FA9-73F3-40F9-8E62-94385CCF4CB1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318B8A87-57F2-4F88-A8FC-AAD66D6BE9AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6465" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="10" r:id="rId1"/>
-    <sheet name="23" sheetId="15" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="18" r:id="rId2"/>
     <sheet name="14" sheetId="16" r:id="rId3"/>
+    <sheet name="23" sheetId="15" r:id="rId4"/>
+    <sheet name="395" sheetId="19" r:id="rId5"/>
+    <sheet name="454" sheetId="17" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="197">
   <si>
     <r>
       <t xml:space="preserve">class </t>
@@ -2774,13 +2777,1824 @@
   </si>
   <si>
     <t xml:space="preserve">approach#2 </t>
+  </si>
+  <si>
+    <t>454. 4Sum II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/4sum-ii/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>fourSumCount(vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&amp; A, vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&amp; B, vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&amp; C, vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&amp; D) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">res = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      unordered_map&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt; map1;</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">      constructMapAB(A, B, map1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      processCD(C, D, map1, res);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>res;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">void </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>constructMapAB(vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&amp; A, vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&amp; B, unordered_map&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt; &amp; map) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">target = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">i = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>; i &lt; A.size(); i++) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">j = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>; j &lt; B.size(); j++) {</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">            target = A[i] + B[j];</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(map.find(target) == map.end()) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">               map[target] = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">else </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>{</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">               map[target]++;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">void </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>processCD(vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&amp; A, vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&amp; B, unordered_map&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&gt; &amp;map, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;res) {</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">            target = -A[i] - B[j];</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(map.find(target) != map.end()) {</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">               res += map[target];</t>
+  </si>
+  <si>
+    <t>//Runtime: 180 ms, faster than 67.58% of C++ online submissions for 4Sum II.</t>
+  </si>
+  <si>
+    <t>//Memory Usage: 28.4 MB, less than 86.36% of C++ online submissions for 4Sum II.</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/longest-substring-with-at-least-k-repeating-characters/</t>
+  </si>
+  <si>
+    <t>395. Longest Substring with At Least K Repeating Characters</t>
+  </si>
+  <si>
+    <t>// Memory Usage : 25.6 MB, less than 27.27% of C++ online submissions for Longest Substring with At Least K Repeating Characters</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">longestSubstring(string s, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>k) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">longestSubstring(s, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, s.length() - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>, k);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">longestSubstring(string &amp;s, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">start, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">end, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>k) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">ans = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">curAns = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(end &lt; start) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt; count(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>256</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>i = start; i &lt;= end; i++) {</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">         count[s[i]]++;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(count[s[i]] != </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;&amp; count[s[i]] &lt; k) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            curAns = longestSubstring(s, start, i - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>, k);</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">            ans = max(ans, curAns);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(ans &gt; end - i) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>ans;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            curAns = longestSubstring(s, i + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>, end, k);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>ans;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">end - start + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>// Memory Usage : 8.8 MB, less than 54.55% of C++ online submissions for Longest Substring with At Least K Repeating Characters.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">int </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>pre = start;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">bool </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">isDivided = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      vector&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt; count(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>26</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">         count[s[i] - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'a'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>]++;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">(count[s[i] - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'a'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">] != </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">0 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">&amp;&amp; count[s[i] - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>'a'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>] &lt; k) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            isDivided = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF660E7A"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(i - pre &gt; ans) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">               curAns = longestSubstring(s, pre, i - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>, k);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">            pre = i + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>(pre &gt; start) {</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">         curAns = longestSubstring(s, pre, end, k);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         ans = max(ans, curAns);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF000080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">isDivided ? ans : end - start + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>二分</t>
+  </si>
+  <si>
+    <t>多分</t>
+  </si>
+  <si>
+    <r>
+      <t>//Runtime:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> 132 ms</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>, faster than 27.86% of C++ online submissions for Longest Substring with At Least K Repeating Characters.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">//Runtime: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>4 ms</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10.5"/>
+        <color rgb="FF808080"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>, faster than 84.94% of C++ online submissions for Longest Substring with At Least K Repeating Characters.</t>
+    </r>
+  </si>
+  <si>
+    <t>多分效率高于二分</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2877,8 +4691,28 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212121"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10.5"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2893,13 +4727,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2932,7 +4760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2950,53 +4778,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3010,6 +4791,47 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3293,124 +5115,149 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A797B7D2-7098-45CE-A64F-08EFFC1E6FA0}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="16.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="27"/>
+    <col min="2" max="2" width="16.28515625" style="28" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="19"/>
+    <col min="5" max="5" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="11">
-        <v>23</v>
-      </c>
-      <c r="C2" s="9" t="str">
+      <c r="B2" s="21">
+        <v>14</v>
+      </c>
+      <c r="C2" s="22" t="str">
         <f ca="1">INDIRECT(B2&amp;"!A1")</f>
-        <v>23. Merge k Sorted Lists</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="20"/>
+        <v>14. Longest Common Prefix</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="20">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="16">
-        <v>14</v>
-      </c>
-      <c r="C3" s="9" t="str">
+      <c r="B3" s="21">
+        <v>23</v>
+      </c>
+      <c r="C3" s="22" t="str">
         <f ca="1">INDIRECT(B3&amp;"!A1")</f>
-        <v>14. Longest Common Prefix</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="21"/>
+        <v>23. Merge k Sorted Lists</v>
+      </c>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="25"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <f t="shared" ref="A4:A8" si="0">A3+1</f>
+      <c r="A4" s="20">
+        <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="22"/>
+      <c r="B4" s="21">
+        <v>395</v>
+      </c>
+      <c r="C4" s="22" t="str">
+        <f ca="1">INDIRECT(B4&amp;"!A1")</f>
+        <v>395. Longest Substring with At Least K Repeating Characters</v>
+      </c>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="25" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
-        <f t="shared" si="0"/>
+      <c r="A5" s="20">
+        <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="23"/>
+      <c r="B5" s="21">
+        <v>454</v>
+      </c>
+      <c r="C5" s="22" t="str">
+        <f ca="1">INDIRECT(B5&amp;"!A1")</f>
+        <v>454. 4Sum II</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <f t="shared" si="0"/>
+      <c r="A6" s="20">
+        <f t="shared" ref="A6:A9" si="0">A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="24"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="20">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="20">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3418,627 +5265,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F89C14-EB96-41AE-ABD4-B3EA5731EAEA}">
-  <dimension ref="A1:D128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC66976-6D2C-47D6-AEAC-EC444E646DD1}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="120.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" s="27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D12" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D20" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D21" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D25" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D26" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D27" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D28" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D29" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D30" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D31" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D32" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D33" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D34" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D35" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D36" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D37" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D41" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D42" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="26"/>
-      <c r="C45" s="26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D46" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D47" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D54" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D55" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D56" s="5"/>
-    </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D57" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D59" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D61" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D62" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D63" s="5"/>
-    </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D64" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D65" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D66" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D67" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D68" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D69" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D70" s="5"/>
-    </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D71" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D72" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D73" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D74" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D76" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D77" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D78" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D79" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D80" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D81" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D82" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D83" s="5"/>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D86" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C89" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D89" s="6"/>
-    </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="6" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D91" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D93" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D94" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D95" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D98" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D99" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D100" s="5"/>
-    </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D101" s="29" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D102" s="5"/>
-    </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D103" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D104" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D105" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D106" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D107" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D108" s="5"/>
-    </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D109" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D110" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D111" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D112" s="4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D113" s="5"/>
-    </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D114" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D115" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D116" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D117" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D118" s="5"/>
-    </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D119" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D120" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D121" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D122" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D123" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D124" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D125" s="5"/>
-    </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{070AF784-3270-4866-9086-A85959998B6D}"/>
-  </hyperlinks>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4053,7 +5287,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="12" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4069,8 +5303,8 @@
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4088,12 +5322,12 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4275,12 +5509,12 @@
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D48" s="27" t="s">
+      <c r="D48" s="8" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="27" t="s">
+      <c r="D49" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4347,6 +5581,1284 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F1C4DB99-34E7-4774-9CDC-C5B8E85C240D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F89C14-EB96-41AE-ABD4-B3EA5731EAEA}">
+  <dimension ref="A1:D128"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="120.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D51" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D53" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="5"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C89" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D89" s="6"/>
+    </row>
+    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D96" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D98" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D99" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D101" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D102" s="5"/>
+    </row>
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D104" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D105" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D106" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D107" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D109" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D110" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D111" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D112" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D113" s="5"/>
+    </row>
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D114" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D115" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D116" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D117" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D119" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D120" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D121" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D122" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D123" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D124" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D125" s="5"/>
+    </row>
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D126" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D127" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D128" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{070AF784-3270-4866-9086-A85959998B6D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D28DDB-F594-4133-A6AE-2DDEEDCA5ECE}">
+  <dimension ref="A1:F84"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="152.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="5"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="5"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D50" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D51" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D53" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D56" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="5"/>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D59" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D60" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D61" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D62" s="5"/>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D64" s="5"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D75" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D77" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B88825FB-BB53-4FCB-BD4E-CEF953E9E4A8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7A18E5-5079-448A-9173-60746C0E3952}">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="108.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{8753C23B-0409-4E9F-ACC8-FE364D1F269A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>

</xml_diff>